<commit_message>
Added Notes test cases Added TaskComment test cases Bug fixes in existing test cases Added BeforeTest / AfterTest methods for parent handling
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData_Lists.xlsx
+++ b/src/main/resources/TestData_Lists.xlsx
@@ -11,21 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>Update</t>
   </si>
   <si>
     <t>My newly created list</t>
   </si>
   <si>
     <t>My second list</t>
-  </si>
-  <si>
-    <t>My newly created second list</t>
   </si>
 </sst>
 </file>
@@ -284,28 +278,22 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.43"/>
+    <col customWidth="1" min="1" max="1" width="23.57"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>